<commit_message>
use 汉字 to mark indicator type
</commit_message>
<xml_diff>
--- a/cases/goodhostpital2021/评价指标体系.xlsx
+++ b/cases/goodhostpital2021/评价指标体系.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="676" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="691" uniqueCount="141">
   <si>
     <t xml:space="preserve">数据名</t>
   </si>
@@ -93,13 +93,13 @@
     <t xml:space="preserve">指标来源</t>
   </si>
   <si>
-    <t xml:space="preserve">三中</t>
-  </si>
-  <si>
-    <t xml:space="preserve">三综</t>
-  </si>
-  <si>
-    <t xml:space="preserve">二综</t>
+    <t xml:space="preserve">三级中医</t>
+  </si>
+  <si>
+    <t xml:space="preserve">三级综合</t>
+  </si>
+  <si>
+    <t xml:space="preserve">二级综合</t>
   </si>
   <si>
     <r>
@@ -130,7 +130,7 @@
     <t xml:space="preserve">新编医院填报</t>
   </si>
   <si>
-    <t xml:space="preserve">-</t>
+    <t xml:space="preserve">自</t>
   </si>
   <si>
     <r>
@@ -178,6 +178,9 @@
     <t xml:space="preserve">自算</t>
   </si>
   <si>
+    <t xml:space="preserve">算</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <sz val="12"/>
@@ -263,7 +266,10 @@
     <t xml:space="preserve">病案首页</t>
   </si>
   <si>
-    <t xml:space="preserve">++</t>
+    <t xml:space="preserve">监</t>
+  </si>
+  <si>
+    <t xml:space="preserve">无</t>
   </si>
   <si>
     <t xml:space="preserve">万元收入能耗占比</t>
@@ -316,7 +322,7 @@
     <t xml:space="preserve">医院填报</t>
   </si>
   <si>
-    <t xml:space="preserve">+</t>
+    <t xml:space="preserve">有</t>
   </si>
   <si>
     <t xml:space="preserve">中医医师占比</t>
@@ -699,7 +705,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -728,6 +734,12 @@
       <name val="PingFang SC"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="PingFang SC"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -772,12 +784,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -801,10 +817,10 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="38" sqref="H2:I4 H8 H13 H16 H23:H24 H27:H29 H32:J33 H42:I42 H44:I44 H49:H50 H53 H61:H63 H68:I68 H70 H83 I9:J11 I13:I14 I18 I20 I24:I26 I35 I47:J47 I49:I52 I55:I57 I59 I62:I63 I72:I75 I79 J2:J5 J7 J14:J15 J17:J22 J25:J27 J35:J38 J41 J51:J59 J66 J71:J81 B2"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="1" sqref="J82 B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.484375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.46875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9"/>
@@ -869,10 +885,10 @@
   <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="38" sqref="H2:I4 H8 H13 H16 H23:H24 H27:H29 H32:J33 H42:I42 H44:I44 H49:H50 H53 H61:H63 H68:I68 H70 H83 I9:J11 I13:I14 I18 I20 I24:I26 I35 I47:J47 I49:I52 I55:I57 I59 I62:I63 I72:I75 I79 J2:J5 J7 J14:J15 J17:J22 J25:J27 J35:J38 J41 J51:J59 J66 J71:J81 C2"/>
+      <selection pane="topLeft" activeCell="C2" activeCellId="1" sqref="J82 C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.484375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.46875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="9"/>
@@ -1040,10 +1056,10 @@
   <dimension ref="A1:J83"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H2" activeCellId="0" sqref="H2:I4 H8 H13 H16 H23:H24 H27:H29 H32:J33 H42:I42 H44:I44 H49:H50 H53 H61:H63 H68:I68 H70 H83 I9:J11 I13:I14 I18 I20 I24:I26 I35 I47:J47 I49:I52 I55:I57 I59 I62:I63 I72:I75 I79 J2:J5 J7 J14:J15 J17:J22 J25:J27 J35:J38 J41 J51:J59 J66 J71:J81"/>
+      <selection pane="topLeft" activeCell="J82" activeCellId="0" sqref="J82"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.484375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.46875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="2" style="0" width="9"/>
@@ -1102,13 +1118,13 @@
       <c r="G2" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="H2" s="0" t="s">
+      <c r="H2" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="I2" s="0" t="s">
+      <c r="I2" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="J2" s="0" t="s">
+      <c r="J2" s="2" t="s">
         <v>29</v>
       </c>
     </row>
@@ -1131,19 +1147,19 @@
       <c r="G3" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="H3" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="I3" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="J3" s="0" t="s">
-        <v>29</v>
+      <c r="H3" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="17.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>10</v>
@@ -1152,24 +1168,24 @@
         <v>3</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="H4" s="0" t="s">
+      <c r="H4" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="I4" s="0" t="s">
+      <c r="I4" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="J4" s="0" t="s">
+      <c r="J4" s="2" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="17.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>17</v>
@@ -1178,27 +1194,27 @@
         <v>3</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="H5" s="0" t="s">
         <v>38</v>
       </c>
-      <c r="I5" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="J5" s="0" t="s">
-        <v>29</v>
+      <c r="H5" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="17.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>15</v>
@@ -1207,27 +1223,27 @@
         <v>3</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="H6" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="I6" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="J6" s="0" t="s">
-        <v>38</v>
+        <v>43</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>9</v>
@@ -1236,27 +1252,27 @@
         <v>1</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="H7" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="I7" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="J7" s="0" t="s">
-        <v>29</v>
+        <v>47</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="17.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>7</v>
@@ -1265,27 +1281,27 @@
         <v>1</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="H8" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="I8" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="J8" s="0" t="s">
-        <v>38</v>
+        <v>50</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="17.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>7</v>
@@ -1294,27 +1310,27 @@
         <v>3</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="H9" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="I9" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="J9" s="0" t="s">
-        <v>29</v>
+        <v>50</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="17.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>15</v>
@@ -1323,27 +1339,27 @@
         <v>3</v>
       </c>
       <c r="E10" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G10" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="F10" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="H10" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="I10" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="J10" s="0" t="s">
-        <v>29</v>
+      <c r="H10" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="17.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>15</v>
@@ -1352,27 +1368,27 @@
         <v>3</v>
       </c>
       <c r="E11" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G11" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="F11" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="H11" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="I11" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="J11" s="0" t="s">
-        <v>29</v>
+      <c r="H11" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="17.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>15</v>
@@ -1381,27 +1397,27 @@
         <v>1</v>
       </c>
       <c r="E12" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G12" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="F12" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="H12" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="I12" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="J12" s="0" t="s">
-        <v>38</v>
+      <c r="H12" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="J12" s="2" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="17.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>14</v>
@@ -1410,27 +1426,27 @@
         <v>3</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="H13" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="I13" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="J13" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="J13" s="2" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="17.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>9</v>
@@ -1439,27 +1455,27 @@
         <v>3</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="H14" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="I14" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="J14" s="0" t="s">
-        <v>29</v>
+        <v>57</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="I14" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="J14" s="2" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="17.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>17</v>
@@ -1468,27 +1484,27 @@
         <v>1</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="H15" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="I15" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="J15" s="0" t="s">
-        <v>29</v>
+        <v>47</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="I15" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="J15" s="2" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="17.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>17</v>
@@ -1497,27 +1513,27 @@
         <v>3</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="H16" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="I16" s="0" t="s">
         <v>38</v>
       </c>
-      <c r="J16" s="0" t="s">
-        <v>38</v>
+      <c r="H16" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="I16" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="J16" s="2" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>9</v>
@@ -1526,27 +1542,27 @@
         <v>1</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="H17" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="I17" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="J17" s="0" t="s">
-        <v>29</v>
+        <v>47</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="I17" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="J17" s="2" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="17.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>15</v>
@@ -1555,27 +1571,27 @@
         <v>3</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="H18" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="I18" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="J18" s="0" t="s">
-        <v>29</v>
+        <v>62</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="J18" s="2" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="17.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>12</v>
@@ -1584,27 +1600,27 @@
         <v>3</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="H19" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="I19" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="J19" s="0" t="s">
-        <v>29</v>
+        <v>47</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="I19" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="J19" s="2" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="17.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>9</v>
@@ -1613,27 +1629,27 @@
         <v>3</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="H20" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="I20" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="J20" s="0" t="s">
-        <v>29</v>
+        <v>57</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="I20" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="J20" s="2" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="17.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>18</v>
@@ -1642,27 +1658,27 @@
         <v>3</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="H21" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="I21" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="J21" s="0" t="s">
-        <v>29</v>
+        <v>43</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="I21" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="J21" s="2" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="17.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>18</v>
@@ -1671,27 +1687,27 @@
         <v>3</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="H22" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="I22" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="J22" s="0" t="s">
-        <v>29</v>
+        <v>43</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="I22" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="J22" s="2" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="17.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>7</v>
@@ -1700,27 +1716,27 @@
         <v>1</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="H23" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="I23" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="J23" s="0" t="s">
-        <v>38</v>
+        <v>50</v>
+      </c>
+      <c r="H23" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="I23" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="J23" s="2" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="17.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>9</v>
@@ -1729,27 +1745,27 @@
         <v>3</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="H24" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="I24" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="J24" s="0" t="s">
         <v>38</v>
+      </c>
+      <c r="H24" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="I24" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="J24" s="2" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="17.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>9</v>
@@ -1758,27 +1774,27 @@
         <v>3</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="H25" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="I25" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="J25" s="0" t="s">
-        <v>29</v>
+        <v>57</v>
+      </c>
+      <c r="H25" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="I25" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="J25" s="2" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="17.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>9</v>
@@ -1787,27 +1803,27 @@
         <v>3</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="H26" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="I26" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="J26" s="0" t="s">
-        <v>29</v>
+        <v>57</v>
+      </c>
+      <c r="H26" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="I26" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="J26" s="2" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="17.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>9</v>
@@ -1816,27 +1832,27 @@
         <v>3</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="H27" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="I27" s="0" t="s">
         <v>38</v>
       </c>
-      <c r="J27" s="0" t="s">
-        <v>29</v>
+      <c r="H27" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="I27" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="J27" s="2" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="17.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>9</v>
@@ -1845,27 +1861,27 @@
         <v>3</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="H28" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="I28" s="0" t="s">
         <v>38</v>
       </c>
-      <c r="J28" s="0" t="s">
-        <v>38</v>
+      <c r="H28" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="I28" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="J28" s="2" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="17.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>9</v>
@@ -1874,27 +1890,27 @@
         <v>3</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="H29" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="I29" s="0" t="s">
         <v>38</v>
       </c>
-      <c r="J29" s="0" t="s">
-        <v>38</v>
+      <c r="H29" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="I29" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="J29" s="2" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="17.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>7</v>
@@ -1903,27 +1919,27 @@
         <v>3</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="H30" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="I30" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="J30" s="0" t="s">
-        <v>38</v>
+        <v>50</v>
+      </c>
+      <c r="H30" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="I30" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="J30" s="2" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="17.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>18</v>
@@ -1932,27 +1948,27 @@
         <v>3</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="H31" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="I31" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="J31" s="0" t="s">
-        <v>38</v>
+        <v>43</v>
+      </c>
+      <c r="H31" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="I31" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="J31" s="2" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="17.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B32" s="0" t="n">
         <v>0.382</v>
@@ -1967,24 +1983,24 @@
         <v>27</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G32" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="H32" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="I32" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="J32" s="0" t="s">
-        <v>29</v>
+      <c r="H32" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="I32" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="J32" s="2" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="17.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="B33" s="0" t="n">
         <v>0.618</v>
@@ -1999,24 +2015,24 @@
         <v>27</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G33" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="H33" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="I33" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="J33" s="0" t="s">
-        <v>29</v>
+      <c r="H33" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="I33" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="J33" s="2" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="17.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>15</v>
@@ -2025,27 +2041,27 @@
         <v>3</v>
       </c>
       <c r="E34" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G34" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="F34" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="G34" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="H34" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="I34" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="J34" s="0" t="s">
-        <v>38</v>
+      <c r="H34" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="I34" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="J34" s="2" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="17.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>15</v>
@@ -2054,27 +2070,27 @@
         <v>3</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="H35" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="I35" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="J35" s="0" t="s">
-        <v>29</v>
+        <v>62</v>
+      </c>
+      <c r="H35" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="I35" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="J35" s="2" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="17.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>8</v>
@@ -2083,27 +2099,27 @@
         <v>1</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="H36" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="I36" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="J36" s="0" t="s">
-        <v>29</v>
+        <v>84</v>
+      </c>
+      <c r="H36" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="I36" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="J36" s="2" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="17.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>8</v>
@@ -2112,27 +2128,27 @@
         <v>1</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="H37" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="I37" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="J37" s="0" t="s">
-        <v>29</v>
+        <v>47</v>
+      </c>
+      <c r="H37" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="I37" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="J37" s="2" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="17.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>8</v>
@@ -2141,27 +2157,27 @@
         <v>1</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="H38" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="I38" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="J38" s="0" t="s">
-        <v>29</v>
+        <v>47</v>
+      </c>
+      <c r="H38" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="I38" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="J38" s="2" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>13</v>
@@ -2175,10 +2191,19 @@
       <c r="G39" s="1" t="s">
         <v>28</v>
       </c>
+      <c r="H39" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="I39" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="J39" s="2" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="40" customFormat="false" ht="17.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>12</v>
@@ -2187,27 +2212,27 @@
         <v>1</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="H40" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="I40" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="J40" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
+      </c>
+      <c r="H40" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="I40" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="J40" s="2" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="17.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>12</v>
@@ -2216,27 +2241,27 @@
         <v>1</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="H41" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="I41" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="J41" s="0" t="s">
-        <v>29</v>
+        <v>91</v>
+      </c>
+      <c r="H41" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="I41" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="J41" s="2" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="17.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>12</v>
@@ -2245,27 +2270,27 @@
         <v>1</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="H42" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="I42" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="J42" s="0" t="s">
-        <v>46</v>
+        <v>93</v>
+      </c>
+      <c r="H42" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="I42" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="J42" s="2" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>13</v>
@@ -2279,10 +2304,19 @@
       <c r="G43" s="1" t="s">
         <v>28</v>
       </c>
+      <c r="H43" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="I43" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="J43" s="2" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>16</v>
@@ -2291,27 +2325,27 @@
         <v>3</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="H44" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="H44" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="I44" s="0" t="s">
+      <c r="I44" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="J44" s="0" t="s">
-        <v>38</v>
+      <c r="J44" s="2" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="17.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>17</v>
@@ -2320,27 +2354,27 @@
         <v>3</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="H45" s="0" t="s">
         <v>38</v>
       </c>
-      <c r="I45" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="J45" s="0" t="s">
-        <v>38</v>
+      <c r="H45" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="I45" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="J45" s="2" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="17.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="1" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>12</v>
@@ -2349,27 +2383,27 @@
         <v>3</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F46" s="0" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="G46" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="H46" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="I46" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="J46" s="0" t="s">
-        <v>38</v>
+        <v>47</v>
+      </c>
+      <c r="H46" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="I46" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="J46" s="2" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="17.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="1" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>7</v>
@@ -2378,27 +2412,27 @@
         <v>3</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G47" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="H47" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="I47" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="J47" s="0" t="s">
-        <v>29</v>
+        <v>47</v>
+      </c>
+      <c r="H47" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="I47" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="J47" s="2" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="17.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="1" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="C48" s="1" t="s">
         <v>15</v>
@@ -2407,27 +2441,27 @@
         <v>3</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G48" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="H48" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="I48" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="J48" s="0" t="s">
-        <v>38</v>
+        <v>43</v>
+      </c>
+      <c r="H48" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="I48" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="J48" s="2" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="17.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="1" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="C49" s="1" t="s">
         <v>18</v>
@@ -2436,27 +2470,27 @@
         <v>3</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G49" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="H49" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="I49" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="J49" s="0" t="s">
-        <v>38</v>
+        <v>43</v>
+      </c>
+      <c r="H49" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="I49" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="J49" s="2" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="17.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="1" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="C50" s="1" t="s">
         <v>18</v>
@@ -2465,27 +2499,27 @@
         <v>3</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G50" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="H50" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="I50" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="J50" s="0" t="s">
-        <v>38</v>
+        <v>43</v>
+      </c>
+      <c r="H50" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="I50" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="J50" s="2" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="1" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="C51" s="1" t="s">
         <v>14</v>
@@ -2494,27 +2528,27 @@
         <v>3</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="G51" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="H51" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="I51" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="J51" s="0" t="s">
-        <v>29</v>
+        <v>47</v>
+      </c>
+      <c r="H51" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="I51" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="J51" s="2" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="1" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C52" s="1" t="s">
         <v>14</v>
@@ -2523,27 +2557,27 @@
         <v>3</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="G52" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="H52" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="I52" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="J52" s="0" t="s">
-        <v>29</v>
+        <v>47</v>
+      </c>
+      <c r="H52" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="I52" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="J52" s="2" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="1" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="C53" s="1" t="s">
         <v>14</v>
@@ -2552,27 +2586,27 @@
         <v>3</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="G53" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="H53" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="I53" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="J53" s="0" t="s">
-        <v>29</v>
+        <v>47</v>
+      </c>
+      <c r="H53" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="I53" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="J53" s="2" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="1" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="C54" s="1" t="s">
         <v>14</v>
@@ -2581,27 +2615,27 @@
         <v>3</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="G54" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="H54" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="I54" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="J54" s="0" t="s">
-        <v>29</v>
+        <v>47</v>
+      </c>
+      <c r="H54" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="I54" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="J54" s="2" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="1" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="C55" s="1" t="s">
         <v>14</v>
@@ -2610,27 +2644,27 @@
         <v>3</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="G55" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="H55" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="I55" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="J55" s="0" t="s">
-        <v>29</v>
+        <v>47</v>
+      </c>
+      <c r="H55" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="I55" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="J55" s="2" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="1" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="C56" s="1" t="s">
         <v>14</v>
@@ -2639,27 +2673,27 @@
         <v>3</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="G56" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="H56" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="I56" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="J56" s="0" t="s">
-        <v>29</v>
+        <v>47</v>
+      </c>
+      <c r="H56" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="I56" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="J56" s="2" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="17.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="1" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="C57" s="1" t="s">
         <v>12</v>
@@ -2668,27 +2702,27 @@
         <v>1</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G57" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="H57" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="I57" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="J57" s="0" t="s">
-        <v>29</v>
+        <v>47</v>
+      </c>
+      <c r="H57" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="I57" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="J57" s="2" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="17.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="1" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="C58" s="1" t="s">
         <v>12</v>
@@ -2697,27 +2731,27 @@
         <v>1</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G58" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="H58" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="I58" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="J58" s="0" t="s">
-        <v>29</v>
+        <v>47</v>
+      </c>
+      <c r="H58" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="I58" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="J58" s="2" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="17.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="1" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="C59" s="1" t="s">
         <v>17</v>
@@ -2726,27 +2760,27 @@
         <v>3</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G59" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="H59" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="I59" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="J59" s="0" t="s">
-        <v>29</v>
+        <v>47</v>
+      </c>
+      <c r="H59" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="I59" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="J59" s="2" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="1" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="C60" s="1" t="s">
         <v>16</v>
@@ -2755,27 +2789,27 @@
         <v>1</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="G60" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="H60" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="I60" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="J60" s="0" t="s">
-        <v>38</v>
+        <v>84</v>
+      </c>
+      <c r="H60" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="I60" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="J60" s="2" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="17.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="1" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="C61" s="1" t="s">
         <v>7</v>
@@ -2784,27 +2818,27 @@
         <v>1</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G61" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="H61" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="I61" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="J61" s="0" t="s">
-        <v>38</v>
+        <v>50</v>
+      </c>
+      <c r="H61" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="I61" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="J61" s="2" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="17.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="1" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="C62" s="1" t="s">
         <v>16</v>
@@ -2813,27 +2847,27 @@
         <v>1</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G62" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="H62" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="I62" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="J62" s="0" t="s">
-        <v>46</v>
+        <v>118</v>
+      </c>
+      <c r="H62" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="I62" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="J62" s="2" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="17.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="1" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="C63" s="1" t="s">
         <v>16</v>
@@ -2842,27 +2876,27 @@
         <v>1</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="F63" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G63" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="H63" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="I63" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="J63" s="0" t="s">
-        <v>46</v>
+        <v>118</v>
+      </c>
+      <c r="H63" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="I63" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="J63" s="2" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="1" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="C64" s="1" t="s">
         <v>13</v>
@@ -2876,10 +2910,19 @@
       <c r="G64" s="1" t="s">
         <v>28</v>
       </c>
+      <c r="H64" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="I64" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="J64" s="2" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="65" customFormat="false" ht="17.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="1" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="C65" s="1" t="s">
         <v>15</v>
@@ -2888,27 +2931,27 @@
         <v>1</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G65" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="H65" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="I65" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="J65" s="0" t="s">
-        <v>38</v>
+        <v>43</v>
+      </c>
+      <c r="H65" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="I65" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="J65" s="2" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="17.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="1" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="C66" s="1" t="s">
         <v>17</v>
@@ -2917,27 +2960,27 @@
         <v>1</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="F66" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G66" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="H66" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="I66" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="J66" s="0" t="s">
-        <v>29</v>
+        <v>84</v>
+      </c>
+      <c r="H66" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="I66" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="J66" s="2" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="1" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="C67" s="1" t="s">
         <v>13</v>
@@ -2951,10 +2994,19 @@
       <c r="G67" s="1" t="s">
         <v>31</v>
       </c>
+      <c r="H67" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="I67" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="J67" s="2" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="68" customFormat="false" ht="17.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="1" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="C68" s="1" t="s">
         <v>12</v>
@@ -2963,27 +3015,27 @@
         <v>3</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G68" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="H68" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="I68" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="J68" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
+      </c>
+      <c r="H68" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="I68" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="J68" s="2" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="17.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="1" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="C69" s="1" t="s">
         <v>12</v>
@@ -2992,27 +3044,27 @@
         <v>3</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="F69" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G69" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="H69" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="I69" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="J69" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
+      </c>
+      <c r="H69" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="I69" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="J69" s="2" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="17.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="1" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="C70" s="1" t="s">
         <v>7</v>
@@ -3021,27 +3073,27 @@
         <v>1</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="F70" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G70" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="H70" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="I70" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="J70" s="0" t="s">
-        <v>38</v>
+        <v>50</v>
+      </c>
+      <c r="H70" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="I70" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="J70" s="2" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="1" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="C71" s="1" t="s">
         <v>9</v>
@@ -3050,27 +3102,27 @@
         <v>1</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="F71" s="1" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="G71" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="H71" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="I71" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="J71" s="0" t="s">
-        <v>29</v>
+        <v>47</v>
+      </c>
+      <c r="H71" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="I71" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="J71" s="2" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="17.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="1" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="C72" s="1" t="s">
         <v>15</v>
@@ -3079,27 +3131,27 @@
         <v>3</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="F72" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G72" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="H72" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="I72" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="J72" s="0" t="s">
-        <v>29</v>
+        <v>62</v>
+      </c>
+      <c r="H72" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="I72" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="J72" s="2" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="17.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="1" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="C73" s="1" t="s">
         <v>9</v>
@@ -3108,27 +3160,27 @@
         <v>3</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="F73" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G73" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="H73" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="I73" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="J73" s="0" t="s">
-        <v>29</v>
+        <v>47</v>
+      </c>
+      <c r="H73" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="I73" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="J73" s="2" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="17.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="1" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="C74" s="1" t="s">
         <v>9</v>
@@ -3137,27 +3189,27 @@
         <v>3</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="F74" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G74" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="H74" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="I74" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="J74" s="0" t="s">
-        <v>29</v>
+        <v>47</v>
+      </c>
+      <c r="H74" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="I74" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="J74" s="2" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="17.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="1" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="C75" s="1" t="s">
         <v>9</v>
@@ -3166,27 +3218,27 @@
         <v>3</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="F75" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G75" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="H75" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="I75" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="J75" s="0" t="s">
-        <v>29</v>
+        <v>47</v>
+      </c>
+      <c r="H75" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="I75" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="J75" s="2" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="17.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="1" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="C76" s="1" t="s">
         <v>12</v>
@@ -3195,27 +3247,27 @@
         <v>3</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="F76" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G76" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="H76" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="I76" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="J76" s="0" t="s">
-        <v>29</v>
+        <v>47</v>
+      </c>
+      <c r="H76" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="I76" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="J76" s="2" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="17.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="1" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="C77" s="1" t="s">
         <v>16</v>
@@ -3224,27 +3276,27 @@
         <v>1</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="F77" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G77" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="H77" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="I77" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="J77" s="0" t="s">
-        <v>29</v>
+        <v>47</v>
+      </c>
+      <c r="H77" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="I77" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="J77" s="2" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="1" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="C78" s="1" t="s">
         <v>16</v>
@@ -3253,27 +3305,27 @@
         <v>1</v>
       </c>
       <c r="E78" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F78" s="1" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="G78" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="H78" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="I78" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="J78" s="0" t="s">
-        <v>29</v>
+        <v>47</v>
+      </c>
+      <c r="H78" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="I78" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="J78" s="2" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="17.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="1" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="C79" s="1" t="s">
         <v>9</v>
@@ -3282,27 +3334,27 @@
         <v>3</v>
       </c>
       <c r="E79" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="F79" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G79" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="H79" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="I79" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="J79" s="0" t="s">
-        <v>29</v>
+        <v>47</v>
+      </c>
+      <c r="H79" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="I79" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="J79" s="2" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="17.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="1" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="C80" s="1" t="s">
         <v>18</v>
@@ -3311,27 +3363,27 @@
         <v>3</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F80" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G80" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="H80" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="I80" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="J80" s="0" t="s">
-        <v>29</v>
+        <v>43</v>
+      </c>
+      <c r="H80" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="I80" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="J80" s="2" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="17.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="1" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="C81" s="1" t="s">
         <v>18</v>
@@ -3340,27 +3392,27 @@
         <v>3</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F81" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G81" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="H81" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="I81" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="J81" s="0" t="s">
-        <v>29</v>
+        <v>43</v>
+      </c>
+      <c r="H81" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="I81" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="J81" s="2" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="1" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="C82" s="1" t="s">
         <v>13</v>
@@ -3369,15 +3421,24 @@
         <v>3</v>
       </c>
       <c r="E82" s="1" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="G82" s="1" t="s">
         <v>28</v>
       </c>
+      <c r="H82" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="I82" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="J82" s="2" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="83" customFormat="false" ht="17.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="1" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="C83" s="1" t="s">
         <v>7</v>
@@ -3386,22 +3447,22 @@
         <v>1</v>
       </c>
       <c r="E83" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="F83" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G83" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="H83" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="I83" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="J83" s="0" t="s">
-        <v>38</v>
+        <v>50</v>
+      </c>
+      <c r="H83" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="I83" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="J83" s="2" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>